<commit_message>
Test case related files
</commit_message>
<xml_diff>
--- a/SeleniumSampleProject/BrowserTests/TestData/UserLogin.xlsx
+++ b/SeleniumSampleProject/BrowserTests/TestData/UserLogin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bharat\Work\Playground\SeleniumExercise\SeleniumSampleProject\BrowserTests\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bharat\Work\Playground\SeleniumExercise\SeleniumAutomationFramework\SeleniumSampleProject\BrowserTests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B6489E-8256-427F-A9C6-626FE5E41ED4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4D84F1-BBE8-47A4-9C7E-EA69E6E07461}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>